<commit_message>
Working logic for text replacement
</commit_message>
<xml_diff>
--- a/ExcelToWord/excelexample.xlsx
+++ b/ExcelToWord/excelexample.xlsx
@@ -24,11 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>ipsum</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <x:si>
+    <x:t>ipsum</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>